<commit_message>
ajustes na funcao de extracao
</commit_message>
<xml_diff>
--- a/tabela_informações_completa_manual_dados_tratados.xlsx
+++ b/tabela_informações_completa_manual_dados_tratados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16-09-2024</t>
+          <t>18-09-2024</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -498,211 +498,211 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Relatório de Correição; Comparativo atualizado; Bizagi Ficha 15, Drive CGMP_RESULTADOS</t>
+          <t>Relatório de Correição</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fls. 11-40, fls. 61-62, fls. 10-10, fls. 11-40</t>
+          <t>fls. 11-40</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Presteza</t>
+          <t>Resolutividade (Produtividade e impacto social)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fichas 15 e 16 do Bizagi, Último Relatório de Correição e Certidão DCOG</t>
+          <t>Comparativo atualizado</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fls. 10-10, fls. 11-40 e fls. 3-4</t>
+          <t>fls. 61-62</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pronto Antedimento</t>
+          <t>Resolutividade (Produtividade e impacto social)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Certidão da DCOG</t>
+          <t>Bizagi Ficha 15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fls. 3-4</t>
+          <t>fls. 10-10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Eficiência</t>
+          <t>Resolutividade (Produtividade e impacto social)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Drive CGMP-Resultados</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fls. 5-6</t>
+          <t>------</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Organização e Desempenho das Funções</t>
+          <t>Presteza</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Fichas 15 e 16 do Bizagi</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fls. 5-6</t>
+          <t>fls. 10-10</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qualidade Técnica</t>
+          <t>Presteza</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Último Relatório de Correição</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fls. 5-6</t>
+          <t>fls. 11-40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Segurança</t>
+          <t>Presteza</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Certidão da DCOG</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fls. 5-6</t>
+          <t>fls. 3-3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Participação em Mutirões e/ou Sessões do Júri</t>
+          <t>Pronto Antedimento</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ficha 6 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Certidão da DCOG</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 3-3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cursos de Formação Continuada</t>
+          <t>Eficiência</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ficha 11 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 5-5</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cursos Oficiais Diversos dos de Formação Continuada e Cursos Reconhecidos de Aperfeiçoamento</t>
+          <t>Organização e Desempenho das Funções</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ficha 12 e 13 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fls. 5-8 e fls. 8-8</t>
+          <t>fls. 5-5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aprimoramento - Doutorado</t>
+          <t>Qualidade Técnica</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 5-5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aprimoramento - Mestrado </t>
+          <t>Segurança</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 3 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 5-5</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Aprimoramento - Especialização</t>
+          <t>Participação em Mutirões e/ou Sessões do Júri</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 6 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -714,12 +714,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Publicações Acadêmicas</t>
+          <t>Cursos de Formação Continuada</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ficha 8 EXTRATO_MERECIMENTO BIZAGI</t>
+          <t>Ficha 11 EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -731,15 +731,117 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Cursos Oficiais Diversos dos de Formação Continuada e Cursos Reconhecidos de Aperfeiçoamento</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ficha 12 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>fls. 6-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Cursos Oficiais Diversos dos de Formação Continuada e Cursos Reconhecidos de Aperfeiçoamento</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ficha 13 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>fls. 8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Aprimoramento - Doutorado</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>fls. 6-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aprimoramento - Mestrado </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>fls. 6-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Aprimoramento - Especialização</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ficha 10 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>fls. 6-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Publicações Acadêmicas</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Ficha 8 EXTRATO_MERECIMENTO BIZAGI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>fls. 6-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>Conduta Profissional e Privada</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>EXTRATO_MERECIMENTO BIZAGI</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>fls. 5-10</t>
         </is>

</xml_diff>

<commit_message>
relatorio de correicao pagina final
</commit_message>
<xml_diff>
--- a/tabela_informações_completa_manual_dados_tratados.xlsx
+++ b/tabela_informações_completa_manual_dados_tratados.xlsx
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18-09-2024</t>
+          <t>23-09-2024</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fls. 11-40</t>
+          <t>fls. 11-64</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fls. 11-40</t>
+          <t>fls. 11-64</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
versao com correcoes de fls
</commit_message>
<xml_diff>
--- a/tabela_informações_completa_manual_dados_tratados.xlsx
+++ b/tabela_informações_completa_manual_dados_tratados.xlsx
@@ -451,16 +451,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10ª PmJ Mossoró</t>
+          <t>PmJ Tangará</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adriana Lira Da Luz Mello</t>
+          <t>Baltazar Patricio Marinho De Figueiredo</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -469,7 +469,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10ª PmJ Mossoró</t>
+          <t>9ª PmJ Parnamirim</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fls. 61-62</t>
+          <t>fls. 65-69</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fls. 10-10</t>
+          <t>fls. 10</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fls. 10-10</t>
+          <t>fls. 10</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fls. 3-3</t>
+          <t>fls. 3-4</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fls. 3-3</t>
+          <t>fls. 3-4</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fls. 5-5</t>
+          <t>fls. 5</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fls. 5-5</t>
+          <t>fls. 5</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fls. 5-5</t>
+          <t>fls. 5</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fls. 5-5</t>
+          <t>fls. 5</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fls. 6-8</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>fls. 8-8</t>
+          <t>fls. 8</t>
         </is>
       </c>
     </row>
@@ -775,7 +775,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -792,7 +792,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>fls. 6-6</t>
+          <t>fls. 6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ajustes no criterio de busca do arquivo 4 - modelo de relatorio alterado
</commit_message>
<xml_diff>
--- a/tabela_informações_completa_manual_dados_tratados.xlsx
+++ b/tabela_informações_completa_manual_dados_tratados.xlsx
@@ -451,25 +451,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PmJ Tangará</t>
+          <t>10ª PmJ Mossoró</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Baltazar Patricio Marinho De Figueiredo</t>
+          <t>Adriana Lira Da Luz Mello</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>23-09-2024</t>
+          <t>18-10-2024</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9ª PmJ Parnamirim</t>
+          <t>10ª PmJ Mossoró</t>
         </is>
       </c>
     </row>
@@ -498,12 +498,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Relatório de Correição</t>
+          <t>Último Relatório de Correição</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fls. 11-64</t>
+          <t>fls. 12-37</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fls. 65-69</t>
+          <t>fls. 56-57</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fls. 10</t>
+          <t>fls. 9</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fls. 10</t>
+          <t>fls. 9</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fls. 11-64</t>
+          <t>fls. 12-37</t>
         </is>
       </c>
     </row>
@@ -724,14 +724,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fls. 6</t>
+          <t>fls. 7</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cursos Oficiais Diversos dos de Formação Continuada e Cursos Reconhecidos de Aperfeiçoamento</t>
+          <t>Cursos Oficiais Diversos dos de Formação Continuada</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -741,14 +741,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fls. 6</t>
+          <t>fls. 7</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cursos Oficiais Diversos dos de Formação Continuada e Cursos Reconhecidos de Aperfeiçoamento</t>
+          <t>Cursos Reconhecidos de Aperfeiçoamento</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">

</xml_diff>